<commit_message>
UM results on raw, original model
</commit_message>
<xml_diff>
--- a/conf/mapping.xlsx
+++ b/conf/mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxspad/proj/nlp-qual-um/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxspad/proj/nlp-qual-um/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86B6163-8F4A-164A-A547-5F50C6D5464A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66E9C5E-37A7-3A4B-AB44-2C3F6E4D027C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{FBD89245-15CD-2644-AEA9-DEC592C5E168}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{FBD89245-15CD-2644-AEA9-DEC592C5E168}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,7 +619,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1179,7 +1179,7 @@
         <v>32</v>
       </c>
       <c r="L14">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>